<commit_message>
Excel without borders for national accounts
</commit_message>
<xml_diff>
--- a/gis/output/all_nominal.xlsx
+++ b/gis/output/all_nominal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au687527\GitHub\GreenGDP\gis\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91474094-98D6-4931-97B4-CFC949B7775D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840E9788-341B-4AF7-A3CC-29B0F555C428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,7 +388,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Excel sheet with nominal cost and investment value (column names merged and bordered)
</commit_message>
<xml_diff>
--- a/gis/output/all_nominal.xlsx
+++ b/gis/output/all_nominal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au687527\GitHub\GreenGDP\gis\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840E9788-341B-4AF7-A3CC-29B0F555C428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3929BF1F-4EEE-4E74-BBF0-511F2A26749C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,6 +25,15 @@
     <t>Cost (current year's prices, million DKK)</t>
   </si>
   <si>
+    <t>Cost (preceding year's prices, million DKK)</t>
+  </si>
+  <si>
+    <t>Investment value (current year's prices, million DKK)</t>
+  </si>
+  <si>
+    <t>Investment value (preceding year's prices, million DKK)</t>
+  </si>
+  <si>
     <t>coastal</t>
   </si>
   <si>
@@ -33,22 +42,21 @@
   <si>
     <t>streams</t>
   </si>
-  <si>
-    <t>Cost (preceding year's prices, million DKK)</t>
-  </si>
-  <si>
-    <t>Investment value (current year's prices, million DKK)</t>
-  </si>
-  <si>
-    <t>Investment value (preceding year's prices, million DKK)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -64,7 +72,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -72,12 +80,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -388,61 +420,71 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -1717,6 +1759,12 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>